<commit_message>
1st full working system
</commit_message>
<xml_diff>
--- a/historical/ADANITRANS.xlsx
+++ b/historical/ADANITRANS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -426,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O149"/>
+  <dimension ref="A1:O150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7435,6 +7435,53 @@
         <v>0.3162</v>
       </c>
     </row>
+    <row r="150" spans="1:15">
+      <c r="A150" s="2">
+        <v>44824</v>
+      </c>
+      <c r="B150" t="s">
+        <v>15</v>
+      </c>
+      <c r="C150" t="s">
+        <v>16</v>
+      </c>
+      <c r="D150">
+        <v>4029.4</v>
+      </c>
+      <c r="E150">
+        <v>4114</v>
+      </c>
+      <c r="F150">
+        <v>4114</v>
+      </c>
+      <c r="G150">
+        <v>3986</v>
+      </c>
+      <c r="H150">
+        <v>3990</v>
+      </c>
+      <c r="I150">
+        <v>4021.55</v>
+      </c>
+      <c r="J150">
+        <v>4048.73</v>
+      </c>
+      <c r="K150">
+        <v>408642</v>
+      </c>
+      <c r="L150">
+        <v>165448049975000</v>
+      </c>
+      <c r="M150">
+        <v>45902</v>
+      </c>
+      <c r="N150">
+        <v>167772</v>
+      </c>
+      <c r="O150">
+        <v>0.4106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>